<commit_message>
updates for tabs and hyperlinks
</commit_message>
<xml_diff>
--- a/Resources/Test12.xlsx
+++ b/Resources/Test12.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\TSU_Excel.suite\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FDB88A-23F0-41BE-BD46-2AD899107341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD07AB72-AFCF-4D43-AC64-68878651F897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="900" windowWidth="28800" windowHeight="15460" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220"/>
   </bookViews>
   <sheets>
     <sheet name="Normalized" sheetId="1" r:id="rId1"/>
     <sheet name="Not Normalized" sheetId="2" r:id="rId2"/>
-    <sheet name="New Worksheet_914000" sheetId="3" r:id="rId6"/>
-    <sheet name="New Worksheet_345000" sheetId="4" r:id="rId7"/>
-    <sheet name="New Worksheet_928000" sheetId="5" r:id="rId8"/>
-    <sheet name="New Worksheet_256000" sheetId="6" r:id="rId9"/>
+    <sheet name="New Worksheet_914000" sheetId="3" r:id="rId3"/>
+    <sheet name="New Worksheet_345000" sheetId="4" r:id="rId4"/>
+    <sheet name="New Worksheet_928000" sheetId="5" r:id="rId5"/>
+    <sheet name="New Worksheet_256000" sheetId="6" r:id="rId6"/>
+    <sheet name="New Worksheet_802000" sheetId="7" r:id="rId7"/>
+    <sheet name="New Worksheet_822000" sheetId="8" r:id="rId8"/>
+    <sheet name="New Worksheet_941000" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -541,9 +544,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08CC13A-FEA9-4C08-B151-AFB39DB95A3A}">
+  <sheetPr>
+    <tabColor rgb="FF00FF00"/>
+  </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -716,9 +722,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A4:E12"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -890,45 +899,106 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
continuing work on hyperlinks
</commit_message>
<xml_diff>
--- a/Resources/Test12.xlsx
+++ b/Resources/Test12.xlsx
@@ -22,6 +22,12 @@
     <sheet name="New Worksheet_802000" sheetId="7" r:id="rId7"/>
     <sheet name="New Worksheet_822000" sheetId="8" r:id="rId8"/>
     <sheet name="New Worksheet_941000" sheetId="9" r:id="rId9"/>
+    <sheet name="New Worksheet_013000" sheetId="10" r:id="rId13"/>
+    <sheet name="New Worksheet_906000" sheetId="11" r:id="rId14"/>
+    <sheet name="New Worksheet_798000" sheetId="12" r:id="rId15"/>
+    <sheet name="New Worksheet_652000" sheetId="13" r:id="rId16"/>
+    <sheet name="New Worksheet_141000" sheetId="14" r:id="rId17"/>
+    <sheet name="New Worksheet_109000" sheetId="15" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -723,6 +729,90 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
   <sheetPr>

</xml_diff>

<commit_message>
testing colors and patterns
</commit_message>
<xml_diff>
--- a/Resources/Test12.xlsx
+++ b/Resources/Test12.xlsx
@@ -28,6 +28,7 @@
     <sheet name="New Worksheet_652000" sheetId="13" r:id="rId16"/>
     <sheet name="New Worksheet_141000" sheetId="14" r:id="rId17"/>
     <sheet name="New Worksheet_109000" sheetId="15" r:id="rId18"/>
+    <sheet name="New Worksheet_691000" sheetId="16" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -813,6 +814,17 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
   <sheetPr>

</xml_diff>

<commit_message>
updated colors and added borders
</commit_message>
<xml_diff>
--- a/Resources/Test12.xlsx
+++ b/Resources/Test12.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,29 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\TSU_Excel.suite\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED44A951-DA40-4572-B266-2EFD7F1B9105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD004732-006B-4E1E-976A-933FBD4A5E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716" activeTab="8"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Normalized" sheetId="1" r:id="rId1"/>
     <sheet name="Not Normalized" sheetId="2" r:id="rId2"/>
-    <sheet name="New Worksheet_914000" sheetId="3" r:id="rId3"/>
-    <sheet name="New Worksheet_345000" sheetId="4" r:id="rId4"/>
-    <sheet name="New Worksheet_928000" sheetId="5" r:id="rId5"/>
-    <sheet name="New Worksheet_256000" sheetId="6" r:id="rId6"/>
-    <sheet name="New Worksheet_802000" sheetId="7" r:id="rId7"/>
-    <sheet name="New Worksheet_822000" sheetId="8" r:id="rId8"/>
-    <sheet name="New Worksheet_941000" sheetId="9" r:id="rId9"/>
-    <sheet name="New Worksheet_013000" sheetId="10" r:id="rId13"/>
-    <sheet name="New Worksheet_906000" sheetId="11" r:id="rId14"/>
-    <sheet name="New Worksheet_798000" sheetId="12" r:id="rId15"/>
-    <sheet name="New Worksheet_652000" sheetId="13" r:id="rId16"/>
-    <sheet name="New Worksheet_141000" sheetId="14" r:id="rId17"/>
-    <sheet name="New Worksheet_109000" sheetId="15" r:id="rId18"/>
-    <sheet name="New Worksheet_691000" sheetId="16" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="79" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
   <si>
     <t>Requirement</t>
   </si>
@@ -156,16 +142,13 @@
   </si>
   <si>
     <t>Spring 2025</t>
-  </si>
-  <si>
-    <t>w</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,21 +187,21 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="right" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -238,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -389,7 +372,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -413,9 +396,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -439,7 +422,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -474,7 +457,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -492,7 +475,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -517,7 +500,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -553,26 +536,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08CC13A-FEA9-4C08-B151-AFB39DB95A3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08CC13A-FEA9-4C08-B151-AFB39DB95A3A}">
   <sheetPr>
     <tabColor rgb="FF00FF00"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,7 +572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -606,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -623,7 +606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -640,7 +623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -657,7 +640,7 @@
         <v>21</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -674,7 +657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -691,7 +674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -708,7 +691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -730,122 +713,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" s="1" customFormat="true" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -879,7 +767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -896,7 +784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -913,7 +801,7 @@
         <v>8</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -930,7 +818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -947,7 +835,7 @@
         <v>21</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -964,7 +852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -981,7 +869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -996,131 +884,6 @@
       </c>
       <c r="E12" t="s">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="B5"/>
-  <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to pattern and borders and adds merge functionality
</commit_message>
<xml_diff>
--- a/Resources/Test12.xlsx
+++ b/Resources/Test12.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,13 +10,15 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD004732-006B-4E1E-976A-933FBD4A5E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716"/>
   </bookViews>
   <sheets>
     <sheet name="Normalized" sheetId="1" r:id="rId1"/>
     <sheet name="Not Normalized" sheetId="2" r:id="rId2"/>
+    <sheet name="New Worksheet_698000" sheetId="3" r:id="rId6"/>
+    <sheet name="New Worksheet_550000" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="78" uniqueCount="34">
   <si>
     <t>Requirement</t>
   </si>
@@ -147,8 +149,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,21 +189,21 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -221,7 +223,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -372,7 +374,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -396,9 +398,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -422,7 +424,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -457,7 +459,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -475,7 +477,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -500,7 +502,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -536,26 +538,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08CC13A-FEA9-4C08-B151-AFB39DB95A3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08CC13A-FEA9-4C08-B151-AFB39DB95A3A}">
   <sheetPr>
     <tabColor rgb="FF00FF00"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -589,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -606,7 +608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -623,7 +625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -640,7 +642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -657,7 +659,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -674,7 +676,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -691,7 +693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -714,7 +716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -724,16 +726,16 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" s="1" customFormat="true" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,7 +752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -767,7 +769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -784,7 +786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -801,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -818,7 +820,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -835,7 +837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -852,7 +854,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -869,7 +871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -889,4 +891,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to object testing and error tracking
</commit_message>
<xml_diff>
--- a/Resources/Test12.xlsx
+++ b/Resources/Test12.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\TSU_Excel.suite\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD004732-006B-4E1E-976A-933FBD4A5E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0240DF-41E9-4D21-A0D9-C425CAF711A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716"/>
   </bookViews>
   <sheets>
     <sheet name="Normalized" sheetId="1" r:id="rId1"/>
-    <sheet name="Not Normalized" sheetId="2" r:id="rId2"/>
-    <sheet name="New Worksheet_698000" sheetId="3" r:id="rId6"/>
-    <sheet name="New Worksheet_550000" sheetId="4" r:id="rId7"/>
+    <sheet name="Copied Worksheet_ 382000" sheetId="4" r:id="rId2"/>
+    <sheet name="Not Normalized" sheetId="2" r:id="rId3"/>
+    <sheet name="New Worksheet_382000" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="117" uniqueCount="34">
   <si>
     <t>Requirement</t>
   </si>
@@ -150,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +166,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -175,7 +193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -183,11 +201,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
@@ -204,6 +243,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,13 +588,189 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08CC13A-FEA9-4C08-B151-AFB39DB95A3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76416718-B7A9-4BEF-B126-C2991CC98B4A}">
   <sheetPr>
-    <tabColor rgb="FF00FF00"/>
+    <tabColor rgb="FF000000"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F01DB-C735-4BB9-88AA-09641D9749E0}">
+  <sheetPr>
+    <tabColor rgb="FF000000"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -715,15 +941,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0C6A51-7AA3-4BA7-BD18-865CAFFC6F6C}">
   <sheetPr>
-    <tabColor rgb="FF0000FF"/>
+    <tabColor rgb="FF000000"/>
   </sheetPr>
   <dimension ref="A4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -893,27 +1119,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D8CA73-A324-4951-A14F-B98E9CCFFBE3}">
   <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
+    <tabColor rgb="FF000000"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update after testing with MYSYS2
minor changes to logging only
</commit_message>
<xml_diff>
--- a/Resources/Test12.xlsx
+++ b/Resources/Test12.xlsx
@@ -1,26 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\TSU_Excel.suite\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0240DF-41E9-4D21-A0D9-C425CAF711A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5D39B5-C5DE-4758-AB66-6062A897D1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Normalized" sheetId="1" r:id="rId1"/>
-    <sheet name="Copied Worksheet_ 125000" sheetId="8" r:id="rId11"/>
-    <sheet name="Copied Worksheet_ 474000" sheetId="6" r:id="rId9"/>
-    <sheet name="Copied Worksheet_ 382000" sheetId="4" r:id="rId2"/>
-    <sheet name="Not Normalized" sheetId="2" r:id="rId3"/>
-    <sheet name="New Worksheet_382000" sheetId="3" r:id="rId4"/>
-    <sheet name="New Worksheet_474000" sheetId="5" r:id="rId8"/>
-    <sheet name="New Worksheet_125000" sheetId="7" r:id="rId10"/>
+    <sheet name="Copied Worksheet_ 698000" sheetId="28" r:id="rId31"/>
+    <sheet name="Copied Worksheet_ 338000" sheetId="26" r:id="rId29"/>
+    <sheet name="Copied Worksheet_ 739000" sheetId="24" r:id="rId27"/>
+    <sheet name="Copied Worksheet_ 866000" sheetId="22" r:id="rId25"/>
+    <sheet name="Copied Worksheet_ 237000" sheetId="20" r:id="rId23"/>
+    <sheet name="Copied Worksheet_ 770000" sheetId="18" r:id="rId21"/>
+    <sheet name="Copied Worksheet_ 716000" sheetId="16" r:id="rId19"/>
+    <sheet name="Copied Worksheet_ 259000" sheetId="14" r:id="rId17"/>
+    <sheet name="Copied Worksheet_ 398000" sheetId="12" r:id="rId15"/>
+    <sheet name="Copied Worksheet_ 620000" sheetId="10" r:id="rId13"/>
+    <sheet name="Copied Worksheet_ 749000" sheetId="8" r:id="rId11"/>
+    <sheet name="Copied Worksheet_ 405000" sheetId="6" r:id="rId9"/>
+    <sheet name="Copied Worksheet_ 413000" sheetId="4" r:id="rId7"/>
+    <sheet name="Not Normalized" sheetId="2" r:id="rId2"/>
+    <sheet name="New Worksheet_413000" sheetId="3" r:id="rId6"/>
+    <sheet name="New Worksheet_405000" sheetId="5" r:id="rId8"/>
+    <sheet name="New Worksheet_749000" sheetId="7" r:id="rId10"/>
+    <sheet name="New Worksheet_620000" sheetId="9" r:id="rId12"/>
+    <sheet name="New Worksheet_398000" sheetId="11" r:id="rId14"/>
+    <sheet name="New Worksheet_259000" sheetId="13" r:id="rId16"/>
+    <sheet name="New Worksheet_716000" sheetId="15" r:id="rId18"/>
+    <sheet name="New Worksheet_770000" sheetId="17" r:id="rId20"/>
+    <sheet name="New Worksheet_237000" sheetId="19" r:id="rId22"/>
+    <sheet name="New Worksheet_866000" sheetId="21" r:id="rId24"/>
+    <sheet name="New Worksheet_739000" sheetId="23" r:id="rId26"/>
+    <sheet name="New Worksheet_338000" sheetId="25" r:id="rId28"/>
+    <sheet name="New Worksheet_698000" sheetId="27" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -43,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="117" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="78" uniqueCount="34">
   <si>
     <t>Requirement</t>
   </si>
@@ -154,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="8">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +226,54 @@
       <b/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -215,7 +283,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -265,11 +333,67 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
@@ -288,7 +412,7 @@
       <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -307,6 +431,38 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -643,13 +799,379 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76416718-B7A9-4BEF-B126-C2991CC98B4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80845A7-30FF-445D-A34E-851B6B1591AB}">
   <sheetPr>
     <tabColor rgb="FF00FF00"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -818,16 +1340,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F01DB-C735-4BB9-88AA-09641D9749E0}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -839,7 +1373,7 @@
   </cols>
   <sheetData>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -996,14 +1530,408 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0C6A51-7AA3-4BA7-BD18-865CAFFC6F6C}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD99B2B-D606-4F6B-94B0-15C4874A4660}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A4:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
@@ -1174,8 +2102,184 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D8CA73-A324-4951-A14F-B98E9CCFFBE3}">
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1183,8 +2287,943 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80845A7-30FF-445D-A34E-851B6B1591AB}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1204,13 +3243,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76416718-B7A9-4BEF-B126-C2991CC98B4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="false" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1222,7 +3261,7 @@
   </cols>
   <sheetData>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1394,13 +3433,13 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76416718-B7A9-4BEF-B126-C2991CC98B4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="false" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1412,7 +3451,7 @@
   </cols>
   <sheetData>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1567,4 +3606,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Retest of TSU scripts
</commit_message>
<xml_diff>
--- a/Resources/Test12.xlsx
+++ b/Resources/Test12.xlsx
@@ -10,10 +10,16 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5D39B5-C5DE-4758-AB66-6062A897D1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716" activeTab="14"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="716" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Normalized" sheetId="1" r:id="rId1"/>
+    <sheet name="Copied Worksheet_ 789000" sheetId="40" r:id="rId43"/>
+    <sheet name="Copied Worksheet_ 578000" sheetId="38" r:id="rId41"/>
+    <sheet name="Copied Worksheet_ 481000" sheetId="36" r:id="rId39"/>
+    <sheet name="Copied Worksheet_ 230000" sheetId="34" r:id="rId37"/>
+    <sheet name="Copied Worksheet_ 832000" sheetId="32" r:id="rId35"/>
+    <sheet name="Copied Worksheet_ 252000" sheetId="30" r:id="rId33"/>
     <sheet name="Copied Worksheet_ 698000" sheetId="28" r:id="rId31"/>
     <sheet name="Copied Worksheet_ 338000" sheetId="26" r:id="rId29"/>
     <sheet name="Copied Worksheet_ 739000" sheetId="24" r:id="rId27"/>
@@ -41,6 +47,12 @@
     <sheet name="New Worksheet_739000" sheetId="23" r:id="rId26"/>
     <sheet name="New Worksheet_338000" sheetId="25" r:id="rId28"/>
     <sheet name="New Worksheet_698000" sheetId="27" r:id="rId30"/>
+    <sheet name="New Worksheet_252000" sheetId="29" r:id="rId32"/>
+    <sheet name="New Worksheet_832000" sheetId="31" r:id="rId34"/>
+    <sheet name="New Worksheet_230000" sheetId="33" r:id="rId36"/>
+    <sheet name="New Worksheet_481000" sheetId="35" r:id="rId38"/>
+    <sheet name="New Worksheet_578000" sheetId="37" r:id="rId40"/>
+    <sheet name="New Worksheet_789000" sheetId="39" r:id="rId42"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -174,7 +186,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="16">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +286,42 @@
       <b/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <b/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -283,7 +331,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -389,11 +437,53 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
@@ -463,6 +553,30 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -817,7 +931,7 @@
   </cols>
   <sheetData>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3038,7 +3152,971 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
@@ -3072,6 +4150,182 @@
   <sheetData>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44870</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45584</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45527</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>